<commit_message>
add 2017 juvy arrest
</commit_message>
<xml_diff>
--- a/new-data/juvenile-arrests/juvenile arrest 2010 to 2017-CLEAN.xlsx
+++ b/new-data/juvenile-arrests/juvenile arrest 2010 to 2017-CLEAN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="426" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="476" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="62">
   <si>
     <t>Year</t>
   </si>
@@ -576,26 +576,26 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Normal_Sheet1" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Weston" xfId="21" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Big Horn" xfId="22" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Campbell" xfId="23" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Crook" xfId="24" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Fremont" xfId="25" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Hot Springs" xfId="26" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Johnson" xfId="27" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Laramie" xfId="28" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Lincoln" xfId="29" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Natrona" xfId="30" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Niobrara" xfId="31" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Park" xfId="32" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Platte" xfId="33" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Sheridan" xfId="34" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Sublette" xfId="35" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Sweetwater" xfId="36" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Teton" xfId="37" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Uinta" xfId="38" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Normal_Washakie" xfId="39" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Sheet1" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Weston" xfId="21" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Big Horn" xfId="22" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Campbell" xfId="23" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Crook" xfId="24" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Fremont" xfId="25" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Hot Springs" xfId="26" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Johnson" xfId="27" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Laramie" xfId="28" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Lincoln" xfId="29" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Natrona" xfId="30" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Niobrara" xfId="31" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Park" xfId="32" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Platte" xfId="33" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Sheridan" xfId="34" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Sublette" xfId="35" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Sweetwater" xfId="36" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Teton" xfId="37" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Uinta" xfId="38" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Excel Built-in Normal_Washakie" xfId="39" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -607,8 +607,8 @@
   </sheetPr>
   <dimension ref="A1:AF65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B185" activeCellId="0" sqref="B185"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A157" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B191" activeCellId="0" sqref="B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16299,101 +16299,101 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B161" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C161" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D161" s="2" t="s">
+      <c r="A161" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B161" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E161" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F161" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G161" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H161" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="I161" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="L161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M161" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O161" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P161" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q161" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S161" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T161" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="U161" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="V161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y161" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA161" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="E161" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F161" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G161" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H161" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I161" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J161" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K161" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L161" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M161" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N161" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O161" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P161" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q161" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R161" s="2" t="s">
+      <c r="AB161" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="S161" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T161" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U161" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V161" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W161" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X161" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y161" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z161" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA161" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB161" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC161" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD161" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE161" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF161" s="2" t="s">
-        <v>31</v>
+      <c r="AC161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE161" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF161" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16401,7 +16401,97 @@
         <v>2017</v>
       </c>
       <c r="B162" s="0" t="s">
-        <v>33</v>
+        <v>39</v>
+      </c>
+      <c r="C162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E162" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F162" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G162" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H162" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="I162" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="L162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M162" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O162" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P162" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="Q162" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S162" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="T162" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="U162" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="V162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X162" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y162" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="Z162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA162" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB162" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE162" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF162" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16409,7 +16499,97 @@
         <v>2017</v>
       </c>
       <c r="B163" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D163" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E163" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F163" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G163" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H163" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="I163" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J163" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K163" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="L163" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M163" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="N163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O163" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P163" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="Q163" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S163" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="T163" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="U163" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="V163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X163" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y163" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="Z163" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA163" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="AB163" s="0" t="n">
+        <v>182</v>
+      </c>
+      <c r="AC163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE163" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF163" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16417,7 +16597,97 @@
         <v>2017</v>
       </c>
       <c r="B164" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H164" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="I164" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K164" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="L164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P164" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q164" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T164" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="U164" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="V164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W164" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X164" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y164" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB164" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE164" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF164" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16425,7 +16695,97 @@
         <v>2017</v>
       </c>
       <c r="B165" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="C165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H165" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="I165" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K165" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="L165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P165" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q165" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T165" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="U165" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="V165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W165" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X165" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y165" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB165" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE165" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF165" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16433,7 +16793,97 @@
         <v>2017</v>
       </c>
       <c r="B166" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G166" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K166" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T166" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U166" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB166" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE166" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF166" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16441,7 +16891,97 @@
         <v>2017</v>
       </c>
       <c r="B167" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="C167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F167" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H167" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="I167" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K167" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="L167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P167" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T167" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="U167" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="V167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X167" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y167" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="Z167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA167" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AB167" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="AC167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD167" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE167" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF167" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16449,7 +16989,97 @@
         <v>2017</v>
       </c>
       <c r="B168" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="C168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F168" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G168" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H168" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="I168" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K168" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="L168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P168" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T168" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="U168" s="0" t="n">
+        <v>48</v>
+      </c>
+      <c r="V168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X168" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y168" s="0" t="n">
+        <v>72</v>
+      </c>
+      <c r="Z168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA168" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB168" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="AC168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD168" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE168" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF168" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16457,7 +17087,97 @@
         <v>2017</v>
       </c>
       <c r="B169" s="0" t="s">
-        <v>45</v>
+        <v>61</v>
+      </c>
+      <c r="C169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F169" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G169" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H169" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="I169" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K169" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="L169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P169" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T169" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="U169" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="V169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X169" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y169" s="0" t="n">
+        <v>74</v>
+      </c>
+      <c r="Z169" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA169" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB169" s="0" t="n">
+        <v>56</v>
+      </c>
+      <c r="AC169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD169" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE169" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF169" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16465,7 +17185,97 @@
         <v>2017</v>
       </c>
       <c r="B170" s="0" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="C170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D170" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F170" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G170" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H170" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="I170" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="J170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K170" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="L170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P170" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="T170" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="U170" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="V170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X170" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y170" s="0" t="n">
+        <v>84</v>
+      </c>
+      <c r="Z170" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA170" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB170" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="AC170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD170" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE170" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF170" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16473,7 +17283,97 @@
         <v>2017</v>
       </c>
       <c r="B171" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="C171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E171" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F171" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="H171" s="0" t="n">
+        <v>82</v>
+      </c>
+      <c r="I171" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K171" s="0" t="n">
+        <v>147</v>
+      </c>
+      <c r="L171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O171" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P171" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q171" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="R171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S171" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="T171" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="U171" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="V171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W171" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="X171" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y171" s="0" t="n">
+        <v>52</v>
+      </c>
+      <c r="Z171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA171" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB171" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="AC171" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD171" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE171" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF171" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16481,7 +17381,97 @@
         <v>2017</v>
       </c>
       <c r="B172" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="C172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D172" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="G172" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I172" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="J172" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K172" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P172" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T172" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X172" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y172" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD172" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE172" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF172" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16489,7 +17479,97 @@
         <v>2017</v>
       </c>
       <c r="B173" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="C173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E173" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F173" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G173" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H173" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="I173" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K173" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="L173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N173" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P173" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q173" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S173" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T173" s="0" t="n">
+        <v>106</v>
+      </c>
+      <c r="U173" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="V173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X173" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y173" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="Z173" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB173" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="AC173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD173" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="AE173" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF173" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16497,7 +17577,97 @@
         <v>2017</v>
       </c>
       <c r="B174" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="C174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E174" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F174" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G174" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H174" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="I174" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K174" s="0" t="n">
+        <v>76</v>
+      </c>
+      <c r="L174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N174" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P174" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q174" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S174" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T174" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="U174" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="V174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X174" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y174" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="Z174" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB174" s="0" t="n">
+        <v>146</v>
+      </c>
+      <c r="AC174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD174" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE174" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF174" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16507,6 +17677,96 @@
       <c r="B175" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="C175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F175" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G175" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H175" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="I175" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K175" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="L175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N175" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O175" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P175" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q175" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S175" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T175" s="0" t="n">
+        <v>120</v>
+      </c>
+      <c r="U175" s="0" t="n">
+        <v>116</v>
+      </c>
+      <c r="V175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X175" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="Y175" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="Z175" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA175" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB175" s="0" t="n">
+        <v>181</v>
+      </c>
+      <c r="AC175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD175" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE175" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF175" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="n">
@@ -16515,6 +17775,96 @@
       <c r="B176" s="0" t="s">
         <v>53</v>
       </c>
+      <c r="C176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D176" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E176" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F176" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G176" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H176" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="I176" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="J176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K176" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="L176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M176" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N176" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O176" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="P176" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q176" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S176" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T176" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="U176" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="V176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="X176" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y176" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="Z176" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA176" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="AB176" s="0" t="n">
+        <v>183</v>
+      </c>
+      <c r="AC176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD176" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE176" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF176" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="n">
@@ -16523,6 +17873,96 @@
       <c r="B177" s="0" t="s">
         <v>54</v>
       </c>
+      <c r="C177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D177" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E177" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F177" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G177" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H177" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="I177" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="J177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K177" s="0" t="n">
+        <v>96</v>
+      </c>
+      <c r="L177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M177" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N177" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O177" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="P177" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q177" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S177" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T177" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="U177" s="0" t="n">
+        <v>145</v>
+      </c>
+      <c r="V177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W177" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X177" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y177" s="0" t="n">
+        <v>132</v>
+      </c>
+      <c r="Z177" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA177" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB177" s="0" t="n">
+        <v>223</v>
+      </c>
+      <c r="AC177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD177" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="AE177" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF177" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="n">
@@ -16531,6 +17971,96 @@
       <c r="B178" s="0" t="s">
         <v>55</v>
       </c>
+      <c r="C178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D178" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E178" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F178" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="G178" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="H178" s="0" t="n">
+        <v>134</v>
+      </c>
+      <c r="I178" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="J178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K178" s="0" t="n">
+        <v>102</v>
+      </c>
+      <c r="L178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M178" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="N178" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="O178" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="P178" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q178" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S178" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T178" s="0" t="n">
+        <v>174</v>
+      </c>
+      <c r="U178" s="0" t="n">
+        <v>170</v>
+      </c>
+      <c r="V178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W178" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="X178" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y178" s="0" t="n">
+        <v>149</v>
+      </c>
+      <c r="Z178" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA178" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="AB178" s="0" t="n">
+        <v>262</v>
+      </c>
+      <c r="AC178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD178" s="0" t="n">
+        <v>68</v>
+      </c>
+      <c r="AE178" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF178" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="n">
@@ -16539,6 +18069,96 @@
       <c r="B179" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="C179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D179" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F179" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G179" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H179" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I179" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J179" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K179" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="L179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P179" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q179" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S179" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T179" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="U179" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="V179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W179" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X179" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y179" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="Z179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA179" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="AB179" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="AC179" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD179" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE179" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF179" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="n">
@@ -16547,6 +18167,96 @@
       <c r="B180" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="C180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D180" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F180" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G180" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H180" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="I180" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J180" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K180" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="L180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P180" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q180" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S180" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T180" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="U180" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="V180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W180" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X180" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y180" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Z180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA180" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB180" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="AC180" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD180" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="AE180" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF180" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="n">
@@ -16555,6 +18265,96 @@
       <c r="B181" s="0" t="s">
         <v>58</v>
       </c>
+      <c r="C181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D181" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F181" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G181" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="H181" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="I181" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J181" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K181" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="L181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P181" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q181" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S181" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T181" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="U181" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="V181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W181" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X181" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y181" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="Z181" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA181" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="AB181" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="AC181" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD181" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE181" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF181" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="n">
@@ -16563,6 +18363,96 @@
       <c r="B182" s="0" t="s">
         <v>59</v>
       </c>
+      <c r="C182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D182" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F182" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G182" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H182" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="I182" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="J182" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K182" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="L182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P182" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q182" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="R182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S182" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T182" s="0" t="n">
+        <v>44</v>
+      </c>
+      <c r="U182" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="V182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W182" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X182" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y182" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="Z182" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA182" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="AB182" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="AC182" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD182" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE182" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF182" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="n">
@@ -16571,7 +18461,122 @@
       <c r="B183" s="0" t="s">
         <v>60</v>
       </c>
+      <c r="C183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="D183" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F183" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="G183" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="H183" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="I183" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="J183" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="K183" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="L183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="M183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="N183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="O183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="P183" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="Q183" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="R183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="S183" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T183" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="U183" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="V183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="W183" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="X183" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y183" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="Z183" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA183" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="AB183" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="AC183" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD183" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE183" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF183" s="0" t="n">
+        <v>0</v>
+      </c>
     </row>
+    <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>